<commit_message>
Adding 27-Apr data and code
</commit_message>
<xml_diff>
--- a/COVID-19/Data/Allformattednumbers.xlsx
+++ b/COVID-19/Data/Allformattednumbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGajula\NotBackedUp\Me\Learn\GitHub\COVID-19\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGajula\NotBackedUp\Me\Learn\GitHub\deepuHub\COVID-19\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="34">
   <si>
     <t>Srikakulam</t>
   </si>
@@ -318,9 +318,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H517"/>
+  <dimension ref="A1:H532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A487" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C513" sqref="C513"/>
+    <sheetView tabSelected="1" topLeftCell="A496" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A519" sqref="A519:F532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -8895,6 +8901,286 @@
         <v>231</v>
       </c>
       <c r="F517" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A519" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B519" s="5">
+        <v>0</v>
+      </c>
+      <c r="C519" s="5">
+        <v>53</v>
+      </c>
+      <c r="D519" s="5">
+        <v>35</v>
+      </c>
+      <c r="E519" s="5">
+        <v>14</v>
+      </c>
+      <c r="F519" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A520" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B520" s="5">
+        <v>0</v>
+      </c>
+      <c r="C520" s="5">
+        <v>73</v>
+      </c>
+      <c r="D520" s="5">
+        <v>57</v>
+      </c>
+      <c r="E520" s="5">
+        <v>16</v>
+      </c>
+      <c r="F520" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A521" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B521" s="5">
+        <v>0</v>
+      </c>
+      <c r="C521" s="5">
+        <v>39</v>
+      </c>
+      <c r="D521" s="5">
+        <v>27</v>
+      </c>
+      <c r="E521" s="5">
+        <v>12</v>
+      </c>
+      <c r="F521" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A522" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B522" s="5">
+        <v>23</v>
+      </c>
+      <c r="C522" s="5">
+        <v>237</v>
+      </c>
+      <c r="D522" s="5">
+        <v>200</v>
+      </c>
+      <c r="E522" s="5">
+        <v>29</v>
+      </c>
+      <c r="F522" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A523" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B523" s="5">
+        <v>0</v>
+      </c>
+      <c r="C523" s="5">
+        <v>58</v>
+      </c>
+      <c r="D523" s="5">
+        <v>30</v>
+      </c>
+      <c r="E523" s="5">
+        <v>28</v>
+      </c>
+      <c r="F523" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A524" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B524" s="5">
+        <v>33</v>
+      </c>
+      <c r="C524" s="5">
+        <v>210</v>
+      </c>
+      <c r="D524" s="5">
+        <v>173</v>
+      </c>
+      <c r="E524" s="5">
+        <v>29</v>
+      </c>
+      <c r="F524" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A525" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B525" s="5">
+        <v>13</v>
+      </c>
+      <c r="C525" s="5">
+        <v>292</v>
+      </c>
+      <c r="D525" s="5">
+        <v>252</v>
+      </c>
+      <c r="E525" s="5">
+        <v>31</v>
+      </c>
+      <c r="F525" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A526" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B526" s="5">
+        <v>7</v>
+      </c>
+      <c r="C526" s="5">
+        <v>79</v>
+      </c>
+      <c r="D526" s="5">
+        <v>54</v>
+      </c>
+      <c r="E526" s="5">
+        <v>23</v>
+      </c>
+      <c r="F526" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A527" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B527" s="5">
+        <v>0</v>
+      </c>
+      <c r="C527" s="5">
+        <v>56</v>
+      </c>
+      <c r="D527" s="5">
+        <v>33</v>
+      </c>
+      <c r="E527" s="5">
+        <v>23</v>
+      </c>
+      <c r="F527" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A528" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B528" s="5">
+        <v>1</v>
+      </c>
+      <c r="C528" s="5">
+        <v>4</v>
+      </c>
+      <c r="D528" s="5">
+        <v>4</v>
+      </c>
+      <c r="E528" s="5">
+        <v>0</v>
+      </c>
+      <c r="F528" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A529" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B529" s="5">
+        <v>0</v>
+      </c>
+      <c r="C529" s="5">
+        <v>22</v>
+      </c>
+      <c r="D529" s="5">
+        <v>3</v>
+      </c>
+      <c r="E529" s="5">
+        <v>19</v>
+      </c>
+      <c r="F529" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A530" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B530" s="5">
+        <v>0</v>
+      </c>
+      <c r="C530" s="5">
+        <v>0</v>
+      </c>
+      <c r="D530" s="5">
+        <v>0</v>
+      </c>
+      <c r="E530" s="5">
+        <v>0</v>
+      </c>
+      <c r="F530" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A531" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B531" s="5">
+        <v>3</v>
+      </c>
+      <c r="C531" s="5">
+        <v>54</v>
+      </c>
+      <c r="D531" s="5">
+        <v>43</v>
+      </c>
+      <c r="E531" s="5">
+        <v>11</v>
+      </c>
+      <c r="F531" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A532" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B532" s="5">
+        <v>80</v>
+      </c>
+      <c r="C532" s="5">
+        <v>1177</v>
+      </c>
+      <c r="D532" s="5">
+        <v>911</v>
+      </c>
+      <c r="E532" s="5">
+        <v>235</v>
+      </c>
+      <c r="F532" s="5">
         <v>31</v>
       </c>
     </row>

</xml_diff>